<commit_message>
fully implement receipts template and update documentation
</commit_message>
<xml_diff>
--- a/LIN, Lee - Gannt Chart (2PAD - 91986 and 91987).xlsx
+++ b/LIN, Lee - Gannt Chart (2PAD - 91986 and 91987).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
     <definedName name="task_start" localSheetId="0">'Project schedule'!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,13 +48,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>Insert new rows ABOVE this one</t>
+    <t xml:space="preserve">Gannt Chart </t>
+  </si>
+  <si>
+    <t>Project start:</t>
+  </si>
+  <si>
+    <t>(2PAD - 91986 and 91987)</t>
+  </si>
+  <si>
+    <t>Display week:</t>
+  </si>
+  <si>
+    <t>TASK</t>
   </si>
   <si>
     <t>PROGRESS</t>
-  </si>
-  <si>
-    <t>Project Management Templates</t>
   </si>
   <si>
     <t>START</t>
@@ -63,66 +72,7 @@
     <t>END</t>
   </si>
   <si>
-    <t>TASK</t>
-  </si>
-  <si>
-    <t>More Project Management Templates</t>
-  </si>
-  <si>
-    <t>About This Template</t>
-  </si>
-  <si>
-    <t>SIMPLE GANTT CHART by Vertex42.com</t>
-  </si>
-  <si>
-    <t>Additional Help</t>
-  </si>
-  <si>
-    <t>About Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortization.</t>
-  </si>
-  <si>
-    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
-  </si>
-  <si>
-    <t>Visit Vertex42.com to download other project management templates, including different types of project schedules, Gantt charts, tasks lists, etc.</t>
-  </si>
-  <si>
-    <t>How to Use the Simple Gantt Chart</t>
-  </si>
-  <si>
-    <t>This template provides a simple way to create a Gantt chart to help visualize and track your project. Simply enter your tasks and start and end dates - no formulas required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
-  </si>
-  <si>
-    <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>There are 2 worksheets in this workbook. 
-TimeSheet
-About
-The instructions for each worksheet are in the A column starting in cell A1 of each worksheet. They are written with hidden text. Each step guides you through the information in that row. Each subsequent step continues in cell A2, A3, and so on, unless otherwise explicitly directed. For example, instruction text might say "continue to cell A6" for the next step. 
-This hidden text will not print.
-To remove these instructions from the worksheet, simply delete column A.</t>
-  </si>
-  <si>
-    <t>Guide for Screen Readers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do not delete this row. This row is hidden to preserve a formula that is used to highlight the current day within the project schedule. </t>
-  </si>
-  <si>
-    <t>Project start:</t>
-  </si>
-  <si>
-    <t>Display week:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gannt Chart </t>
-  </si>
-  <si>
-    <t>(2PAD - 91986 and 91987)</t>
   </si>
   <si>
     <t>Set up / Planning and design</t>
@@ -148,21 +98,71 @@
   <si>
     <t>Research Version Control</t>
   </si>
+  <si>
+    <t>Insert new rows ABOVE this one</t>
+  </si>
+  <si>
+    <t>SIMPLE GANTT CHART by Vertex42.com</t>
+  </si>
+  <si>
+    <t>About This Template</t>
+  </si>
+  <si>
+    <t>This template provides a simple way to create a Gantt chart to help visualize and track your project. Simply enter your tasks and start and end dates - no formulas required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
+  </si>
+  <si>
+    <t>Guide for Screen Readers</t>
+  </si>
+  <si>
+    <t>There are 2 worksheets in this workbook. 
+TimeSheet
+About
+The instructions for each worksheet are in the A column starting in cell A1 of each worksheet. They are written with hidden text. Each step guides you through the information in that row. Each subsequent step continues in cell A2, A3, and so on, unless otherwise explicitly directed. For example, instruction text might say "continue to cell A6" for the next step. 
+This hidden text will not print.
+To remove these instructions from the worksheet, simply delete column A.</t>
+  </si>
+  <si>
+    <t>Additional Help</t>
+  </si>
+  <si>
+    <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
+  </si>
+  <si>
+    <t>How to Use the Simple Gantt Chart</t>
+  </si>
+  <si>
+    <t>More Project Management Templates</t>
+  </si>
+  <si>
+    <t>Visit Vertex42.com to download other project management templates, including different types of project schedules, Gantt charts, tasks lists, etc.</t>
+  </si>
+  <si>
+    <t>Project Management Templates</t>
+  </si>
+  <si>
+    <t>About Vertex42</t>
+  </si>
+  <si>
+    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortization.</t>
+  </si>
+  <si>
+    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
-    <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="168" formatCode="d"/>
-    <numFmt numFmtId="169" formatCode="d/mm/yy;@"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="d"/>
+    <numFmt numFmtId="168" formatCode="d/mm/yy;@"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -710,7 +710,7 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -719,10 +719,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" applyFill="0">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyFill="0">
@@ -804,13 +804,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="21" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="21" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="21" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,7 +838,7 @@
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,7 +922,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -934,10 +934,10 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -973,94 +973,94 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="3" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="169" fontId="19" fillId="3" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="3" borderId="7" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="169" fontId="19" fillId="3" borderId="7" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="8" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="169" fontId="19" fillId="8" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="3" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="19" fillId="3" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1465,10 +1465,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1677,11 +1673,11 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.75" style="13" customWidth="1"/>
     <col min="2" max="2" width="22.75" customWidth="1"/>
@@ -1694,175 +1690,175 @@
     <col min="9" max="65" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.1000000000000001">
+    <row r="1" spans="1:64" ht="90" customHeight="1">
       <c r="A1" s="14"/>
       <c r="B1" s="80" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="106" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
+      <c r="I1" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="104">
+      <c r="Q1" s="111">
         <v>45778</v>
       </c>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1">
       <c r="B2" s="78" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C2" s="79"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="106" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
+      <c r="I2" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="102">
+      <c r="Q2" s="110">
         <v>1</v>
       </c>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-    </row>
-    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+    </row>
+    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="25"/>
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="29"/>
       <c r="E4" s="30"/>
-      <c r="I4" s="99">
+      <c r="I4" s="115">
         <f>I5</f>
         <v>45775</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97">
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113">
         <f>P5</f>
         <v>45782</v>
       </c>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97">
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="113">
         <f>W5</f>
         <v>45789</v>
       </c>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97">
+      <c r="X4" s="113"/>
+      <c r="Y4" s="113"/>
+      <c r="Z4" s="113"/>
+      <c r="AA4" s="113"/>
+      <c r="AB4" s="113"/>
+      <c r="AC4" s="113"/>
+      <c r="AD4" s="113">
         <f>AD5</f>
         <v>45796</v>
       </c>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="97">
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="113"/>
+      <c r="AG4" s="113"/>
+      <c r="AH4" s="113"/>
+      <c r="AI4" s="113"/>
+      <c r="AJ4" s="113"/>
+      <c r="AK4" s="113">
         <f>AK5</f>
         <v>45803</v>
       </c>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="97">
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="113"/>
+      <c r="AN4" s="113"/>
+      <c r="AO4" s="113"/>
+      <c r="AP4" s="113"/>
+      <c r="AQ4" s="113"/>
+      <c r="AR4" s="113">
         <f>AR5</f>
         <v>45810</v>
       </c>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="97"/>
-      <c r="AU4" s="97"/>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="97">
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="113"/>
+      <c r="AU4" s="113"/>
+      <c r="AV4" s="113"/>
+      <c r="AW4" s="113"/>
+      <c r="AX4" s="113"/>
+      <c r="AY4" s="113">
         <f>AY5</f>
         <v>45817</v>
       </c>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="97"/>
-      <c r="BB4" s="97"/>
-      <c r="BC4" s="97"/>
-      <c r="BD4" s="97"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="97">
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="113"/>
+      <c r="BB4" s="113"/>
+      <c r="BC4" s="113"/>
+      <c r="BD4" s="113"/>
+      <c r="BE4" s="113"/>
+      <c r="BF4" s="113">
         <f>BF5</f>
         <v>45824</v>
       </c>
-      <c r="BG4" s="97"/>
-      <c r="BH4" s="97"/>
-      <c r="BI4" s="97"/>
-      <c r="BJ4" s="97"/>
-      <c r="BK4" s="97"/>
-      <c r="BL4" s="98"/>
-    </row>
-    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="108"/>
-      <c r="B5" s="109" t="s">
+      <c r="BG4" s="113"/>
+      <c r="BH4" s="113"/>
+      <c r="BI4" s="113"/>
+      <c r="BJ4" s="113"/>
+      <c r="BK4" s="113"/>
+      <c r="BL4" s="114"/>
+    </row>
+    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="105"/>
+      <c r="B5" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="100" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="100" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="100" t="s">
-        <v>4</v>
+      <c r="E5" s="109" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="109" t="s">
+        <v>7</v>
       </c>
       <c r="I5" s="31">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
@@ -2089,13 +2085,13 @@
         <v>45830</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="105"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
       <c r="I6" s="34" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2321,9 +2317,9 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="38"/>
@@ -2331,7 +2327,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="H7" s="26" t="str">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="39"/>
@@ -2391,10 +2387,10 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -2402,7 +2398,7 @@
       <c r="F8" s="94"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H34" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H34" ca="1" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2462,10 +2458,10 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="14"/>
       <c r="B9" s="46" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="48">
@@ -2481,7 +2477,7 @@
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="I9" s="49"/>
@@ -2541,10 +2537,10 @@
       <c r="BK9" s="49"/>
       <c r="BL9" s="49"/>
     </row>
-    <row r="10" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A10" s="14"/>
       <c r="B10" s="46" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="48">
@@ -2615,10 +2611,10 @@
       <c r="BK10" s="49"/>
       <c r="BL10" s="49"/>
     </row>
-    <row r="11" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="14"/>
       <c r="B11" s="50" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C11" s="51"/>
       <c r="D11" s="52">
@@ -2633,7 +2629,7 @@
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>3</v>
       </c>
       <c r="I11" s="49"/>
@@ -2693,10 +2689,10 @@
       <c r="BK11" s="49"/>
       <c r="BL11" s="49"/>
     </row>
-    <row r="12" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A12" s="13"/>
       <c r="B12" s="50" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C12" s="51"/>
       <c r="D12" s="52">
@@ -2712,7 +2708,7 @@
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>6</v>
       </c>
       <c r="I12" s="49"/>
@@ -2772,10 +2768,10 @@
       <c r="BK12" s="49"/>
       <c r="BL12" s="49"/>
     </row>
-    <row r="13" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="13"/>
       <c r="B13" s="46" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C13" s="47"/>
       <c r="D13" s="48">
@@ -2789,7 +2785,7 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="I13" s="49"/>
@@ -2849,10 +2845,10 @@
       <c r="BK13" s="49"/>
       <c r="BL13" s="49"/>
     </row>
-    <row r="14" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A14" s="13"/>
       <c r="B14" s="50" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C14" s="51"/>
       <c r="D14" s="52">
@@ -2866,7 +2862,7 @@
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="I14" s="49"/>
@@ -2926,24 +2922,24 @@
       <c r="BK14" s="49"/>
       <c r="BL14" s="49"/>
     </row>
-    <row r="15" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="14"/>
       <c r="G15" s="17"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="14"/>
       <c r="B16" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="113">
+        <v>16</v>
+      </c>
+      <c r="C16" s="97"/>
+      <c r="D16" s="98">
         <v>1</v>
       </c>
-      <c r="E16" s="114">
+      <c r="E16" s="99">
         <v>45793</v>
       </c>
-      <c r="F16" s="115">
+      <c r="F16" s="100">
         <v>45794</v>
       </c>
       <c r="G16" s="17"/>
@@ -2966,8 +2962,8 @@
       <c r="X16" s="49"/>
       <c r="Y16" s="49"/>
       <c r="Z16" s="49"/>
-      <c r="AA16" s="119"/>
-      <c r="AB16" s="119"/>
+      <c r="AA16" s="104"/>
+      <c r="AB16" s="104"/>
       <c r="AC16" s="49"/>
       <c r="AD16" s="49"/>
       <c r="AE16" s="49"/>
@@ -3004,13 +3000,13 @@
       <c r="BK16" s="49"/>
       <c r="BL16" s="49"/>
     </row>
-    <row r="17" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="50"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="17"/>
       <c r="H17" s="5"/>
       <c r="I17" s="49"/>
@@ -3070,13 +3066,13 @@
       <c r="BK17" s="49"/>
       <c r="BL17" s="49"/>
     </row>
-    <row r="18" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A18" s="13"/>
       <c r="B18" s="50"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
       <c r="G18" s="17"/>
       <c r="H18" s="5"/>
       <c r="I18" s="49"/>
@@ -3136,13 +3132,13 @@
       <c r="BK18" s="49"/>
       <c r="BL18" s="49"/>
     </row>
-    <row r="19" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="13"/>
       <c r="B19" s="50"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
       <c r="G19" s="17"/>
       <c r="H19" s="5"/>
       <c r="I19" s="49"/>
@@ -3202,13 +3198,13 @@
       <c r="BK19" s="49"/>
       <c r="BL19" s="49"/>
     </row>
-    <row r="20" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="13"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
       <c r="G20" s="17"/>
       <c r="H20" s="5"/>
       <c r="I20" s="49"/>
@@ -3268,7 +3264,7 @@
       <c r="BK20" s="49"/>
       <c r="BL20" s="49"/>
     </row>
-    <row r="21" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="13"/>
       <c r="B21" s="54"/>
       <c r="C21" s="55"/>
@@ -3334,7 +3330,7 @@
       <c r="BK21" s="57"/>
       <c r="BL21" s="57"/>
     </row>
-    <row r="22" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A22" s="13"/>
       <c r="B22" s="58"/>
       <c r="C22" s="59"/>
@@ -3400,7 +3396,7 @@
       <c r="BK22" s="49"/>
       <c r="BL22" s="49"/>
     </row>
-    <row r="23" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="13"/>
       <c r="B23" s="58"/>
       <c r="C23" s="59"/>
@@ -3466,7 +3462,7 @@
       <c r="BK23" s="49"/>
       <c r="BL23" s="49"/>
     </row>
-    <row r="24" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A24" s="13"/>
       <c r="B24" s="58"/>
       <c r="C24" s="59"/>
@@ -3532,7 +3528,7 @@
       <c r="BK24" s="49"/>
       <c r="BL24" s="49"/>
     </row>
-    <row r="25" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -3598,7 +3594,7 @@
       <c r="BK25" s="49"/>
       <c r="BL25" s="49"/>
     </row>
-    <row r="26" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A26" s="13"/>
       <c r="B26" s="58"/>
       <c r="C26" s="59"/>
@@ -3664,7 +3660,7 @@
       <c r="BK26" s="49"/>
       <c r="BL26" s="49"/>
     </row>
-    <row r="27" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="13"/>
       <c r="B27" s="61"/>
       <c r="C27" s="62"/>
@@ -3730,7 +3726,7 @@
       <c r="BK27" s="64"/>
       <c r="BL27" s="64"/>
     </row>
-    <row r="28" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="13"/>
       <c r="B28" s="65"/>
       <c r="C28" s="66"/>
@@ -3796,7 +3792,7 @@
       <c r="BK28" s="49"/>
       <c r="BL28" s="49"/>
     </row>
-    <row r="29" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="13"/>
       <c r="B29" s="65"/>
       <c r="C29" s="66"/>
@@ -3862,7 +3858,7 @@
       <c r="BK29" s="49"/>
       <c r="BL29" s="49"/>
     </row>
-    <row r="30" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A30" s="13"/>
       <c r="B30" s="65"/>
       <c r="C30" s="66"/>
@@ -3928,7 +3924,7 @@
       <c r="BK30" s="49"/>
       <c r="BL30" s="49"/>
     </row>
-    <row r="31" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A31" s="13"/>
       <c r="B31" s="65"/>
       <c r="C31" s="66"/>
@@ -3994,7 +3990,7 @@
       <c r="BK31" s="49"/>
       <c r="BL31" s="49"/>
     </row>
-    <row r="32" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A32" s="13"/>
       <c r="B32" s="65"/>
       <c r="C32" s="66"/>
@@ -4060,7 +4056,7 @@
       <c r="BK32" s="49"/>
       <c r="BL32" s="49"/>
     </row>
-    <row r="33" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A33" s="13"/>
       <c r="B33" s="68"/>
       <c r="C33" s="69"/>
@@ -4126,10 +4122,10 @@
       <c r="BK33" s="44"/>
       <c r="BL33" s="44"/>
     </row>
-    <row r="34" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A34" s="14"/>
       <c r="B34" s="72" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C34" s="73"/>
       <c r="D34" s="74"/>
@@ -4137,7 +4133,7 @@
       <c r="F34" s="76"/>
       <c r="G34" s="17"/>
       <c r="H34" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="I34" s="77"/>
@@ -4197,28 +4193,18 @@
       <c r="BK34" s="77"/>
       <c r="BL34" s="77"/>
     </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" ht="30" customHeight="1">
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:64" ht="30" customHeight="1">
       <c r="C36" s="16"/>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" ht="30" customHeight="1">
       <c r="C37" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4227,6 +4213,16 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D14 D16:D34">
     <cfRule type="dataBar" priority="23">
@@ -4337,110 +4333,110 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="87" style="7" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.75">
       <c r="A2" s="81" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="82"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="31.5">
       <c r="A4" s="83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="74.25" customHeight="1">
       <c r="A5" s="84" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" customHeight="1">
       <c r="A6" s="83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1">
       <c r="A7" s="85" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="31.5">
       <c r="A8" s="83" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="57">
       <c r="A9" s="84" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1">
       <c r="A10" s="86" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="31.5">
       <c r="A11" s="83" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.5">
       <c r="A12" s="84" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1">
       <c r="A13" s="86" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="10" customFormat="1" ht="31.5">
       <c r="A14" s="83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="75" customHeight="1">
       <c r="A15" s="84" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="71.25">
       <c r="A16" s="84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="87"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="87"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="87"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="87"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="87"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="87"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="87"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="87"/>
     </row>
   </sheetData>
@@ -4456,23 +4452,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4788,60 +4773,35 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>